<commit_message>
reddit: Fix reddit comment retrieval
</commit_message>
<xml_diff>
--- a/SocialMediaAnalysis/inputData.xlsx
+++ b/SocialMediaAnalysis/inputData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjak923\Documents\social-media-analysis\SocialMediaAnalysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FA82EC-E58C-4D3C-8652-664BEB733842}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7471B6-990B-4274-BA59-DB9AE126E0D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2295" yWindow="2295" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>